<commit_message>
Update SlicerRT users table
</commit_message>
<xml_diff>
--- a/overview/SlicerRT_Users.xlsx
+++ b/overview/SlicerRT_Users.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="208">
   <si>
     <t>User</t>
   </si>
@@ -608,9 +608,6 @@
     <t>Room's Eye View with Siemens linac</t>
   </si>
   <si>
-    <t>Madrid, Spain</t>
-  </si>
-  <si>
     <t>Roozbeh Shams</t>
   </si>
   <si>
@@ -663,6 +660,9 @@
   </si>
   <si>
     <t>Hohmann.Stephan@mayo.edu</t>
+  </si>
+  <si>
+    <t>Hospital Universitario de Fuenlabrada, Madrid, Spain</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1055,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,7 +1412,7 @@
         <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>74</v>
@@ -1486,7 +1486,7 @@
         <v>90</v>
       </c>
       <c r="C29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>91</v>
@@ -1860,10 +1860,13 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>201</v>
+        <v>200</v>
+      </c>
+      <c r="B50" t="s">
+        <v>197</v>
       </c>
       <c r="C50" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>187</v>
@@ -1877,16 +1880,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B51" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C51" t="s">
         <v>182</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F51" s="3">
         <v>43220</v>
@@ -1894,33 +1897,33 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>191</v>
+      </c>
+      <c r="B52" t="s">
+        <v>193</v>
+      </c>
+      <c r="C52" t="s">
+        <v>193</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="B52" t="s">
-        <v>194</v>
-      </c>
-      <c r="C52" t="s">
-        <v>194</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>196</v>
+      </c>
+      <c r="B53" t="s">
         <v>197</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>198</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="E53" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F53" s="3">
         <v>43378</v>
@@ -1928,19 +1931,19 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>203</v>
+      </c>
+      <c r="B54" t="s">
         <v>204</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
+        <v>202</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E54" t="s">
         <v>205</v>
-      </c>
-      <c r="C54" t="s">
-        <v>203</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E54" t="s">
-        <v>206</v>
       </c>
       <c r="F54" s="3">
         <v>43396</v>

</xml_diff>